<commit_message>
fix plot head angular speed script to include taking angle difference, also wrote several functions and tidied up script using functions
</commit_message>
<xml_diff>
--- a/datalists/N2_40_g_list_hamm.xlsx
+++ b/datalists/N2_40_g_list_hamm.xlsx
@@ -374,12 +374,12 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="69" customWidth="1"/>
+    <col min="1" max="1" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>